<commit_message>
Update DigiKey BOM for Hyperboard
</commit_message>
<xml_diff>
--- a/notes/Hyperboard/AVIELF2HYPERBOARD-BOM.xlsx
+++ b/notes/Hyperboard/AVIELF2HYPERBOARD-BOM.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/andrewwasson/Development/avi-elf-ii/notes/Hyperboard/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{980A2D8A-99E9-4F4D-83C8-1D4BB75E0922}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{62C951AE-3A03-8043-8A47-AFA3795FF986}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22360" yWindow="8220" windowWidth="37800" windowHeight="20080" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -112,9 +112,6 @@
     <t>LED</t>
   </si>
   <si>
-    <t>D9, D10, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21</t>
-  </si>
-  <si>
     <t>1N914</t>
   </si>
   <si>
@@ -542,6 +539,9 @@
   </si>
   <si>
     <t>https://www.digikey.com/en/products/detail/adam-tech/PH2-80-UA/9830504</t>
+  </si>
+  <si>
+    <t>D9, D10, D11, D12, D13, D14, D15, D16, D17, D18, D19, D20, D21</t>
   </si>
 </sst>
 </file>
@@ -1444,8 +1444,8 @@
 <worksheet xmlns="http://purl.oclc.org/ooxml/spreadsheetml/main" xmlns:r="http://purl.oclc.org/ooxml/officeDocument/relationships" xmlns:v="urn:schemas-microsoft-com:vml" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A12" workbookViewId="0">
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1460,27 +1460,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -1489,16 +1489,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -1515,10 +1515,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -1535,10 +1535,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -1555,10 +1555,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -1572,13 +1572,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
+        <v>67</v>
+      </c>
+      <c r="F7" s="4" t="s">
         <v>68</v>
-      </c>
-      <c r="F7" s="4" t="s">
-        <v>69</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -1589,13 +1589,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
+        <v>73</v>
+      </c>
+      <c r="F8" s="4" t="s">
         <v>74</v>
-      </c>
-      <c r="F8" s="4" t="s">
-        <v>75</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -1606,13 +1606,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
+        <v>75</v>
+      </c>
+      <c r="F9" s="4" t="s">
         <v>76</v>
-      </c>
-      <c r="F9" s="4" t="s">
-        <v>77</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -1623,13 +1623,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
+        <v>77</v>
+      </c>
+      <c r="F10" s="4" t="s">
         <v>78</v>
-      </c>
-      <c r="F10" s="4" t="s">
-        <v>79</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -1640,13 +1640,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
         <v>80</v>
       </c>
-      <c r="D11" t="s">
+      <c r="F11" s="4" t="s">
         <v>81</v>
-      </c>
-      <c r="F11" s="4" t="s">
-        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -1657,13 +1657,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="D12" t="s">
+        <v>82</v>
+      </c>
+      <c r="F12" s="4" t="s">
         <v>84</v>
-      </c>
-      <c r="D12" t="s">
-        <v>83</v>
-      </c>
-      <c r="F12" s="4" t="s">
-        <v>85</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -1674,13 +1674,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" t="s">
+      <c r="F13" s="4" t="s">
         <v>87</v>
-      </c>
-      <c r="F13" s="4" t="s">
-        <v>88</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -1694,10 +1694,10 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
+        <v>88</v>
+      </c>
+      <c r="F14" s="4" t="s">
         <v>89</v>
-      </c>
-      <c r="F14" s="4" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -1711,10 +1711,10 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -1725,35 +1725,35 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D20" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="F20" s="4" t="s">
         <v>54</v>
-      </c>
-      <c r="F20" s="4" t="s">
-        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -1761,16 +1761,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D21" t="s">
+        <v>95</v>
+      </c>
+      <c r="F21" s="4" t="s">
         <v>96</v>
-      </c>
-      <c r="F21" s="4" t="s">
-        <v>97</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -1778,16 +1778,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="D22" t="s">
+        <v>97</v>
+      </c>
+      <c r="F22" s="4" t="s">
         <v>99</v>
-      </c>
-      <c r="D22" t="s">
-        <v>98</v>
-      </c>
-      <c r="F22" s="4" t="s">
-        <v>100</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -1796,7 +1796,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24" s="4"/>
@@ -1812,13 +1812,13 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -1827,7 +1827,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3"/>
       <c r="F27" s="4"/>
@@ -1840,13 +1840,13 @@
         <v>20</v>
       </c>
       <c r="C28" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="D28" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="F28" s="4" t="s">
         <v>104</v>
-      </c>
-      <c r="D28" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="F28" s="4" t="s">
-        <v>105</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -1860,10 +1860,10 @@
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -1874,13 +1874,13 @@
         <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -1891,13 +1891,13 @@
         <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="3" t="s">
+      <c r="F31" s="4" t="s">
         <v>112</v>
-      </c>
-      <c r="F31" s="4" t="s">
-        <v>113</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -1908,18 +1908,18 @@
         <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D32" s="3" t="s">
+      <c r="F32" s="12" t="s">
         <v>115</v>
-      </c>
-      <c r="F32" s="12" t="s">
-        <v>116</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -1927,16 +1927,16 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D35" t="s">
+        <v>116</v>
+      </c>
+      <c r="F35" s="4" t="s">
         <v>117</v>
-      </c>
-      <c r="F35" s="4" t="s">
-        <v>118</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -1944,16 +1944,16 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -1961,16 +1961,16 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D37" t="s">
+        <v>120</v>
+      </c>
+      <c r="F37" s="4" t="s">
         <v>121</v>
-      </c>
-      <c r="F37" s="4" t="s">
-        <v>122</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -1978,16 +1978,16 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -1995,16 +1995,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D39" t="s">
+        <v>124</v>
+      </c>
+      <c r="F39" s="4" t="s">
         <v>125</v>
-      </c>
-      <c r="F39" s="4" t="s">
-        <v>126</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2012,16 +2012,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D40" t="s">
+        <v>126</v>
+      </c>
+      <c r="F40" s="4" t="s">
         <v>127</v>
-      </c>
-      <c r="F40" s="4" t="s">
-        <v>128</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2029,16 +2029,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3">
         <v>100</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2046,16 +2046,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2063,16 +2063,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="3">
         <v>470</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2080,19 +2080,19 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D45" s="13" t="s">
+        <v>134</v>
+      </c>
+      <c r="E45" s="14" t="s">
+        <v>138</v>
+      </c>
+      <c r="F45" s="4" t="s">
         <v>135</v>
-      </c>
-      <c r="E45" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="F45" s="4" t="s">
-        <v>136</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2100,19 +2100,19 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D46" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E46" s="14" t="s">
-        <v>139</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
     </row>
   </sheetData>
@@ -2155,7 +2155,7 @@
   <dimension ref="A1:F46"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="A21" sqref="A21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2170,27 +2170,27 @@
   <sheetData>
     <row r="1" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>49</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>50</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>52</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:6" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A2" s="6" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C2" s="2"/>
     </row>
@@ -2199,16 +2199,16 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="E3" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F3" t="s">
         <v>17</v>
@@ -2225,10 +2225,10 @@
         <v>1</v>
       </c>
       <c r="D4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E4" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F4" t="s">
         <v>17</v>
@@ -2245,10 +2245,10 @@
         <v>3</v>
       </c>
       <c r="D5" s="9" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F5" t="s">
         <v>17</v>
@@ -2265,10 +2265,10 @@
         <v>16</v>
       </c>
       <c r="D6" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E6" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="F6" t="s">
         <v>17</v>
@@ -2282,13 +2282,13 @@
         <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="D7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -2299,13 +2299,13 @@
         <v>18</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="D8" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="F8" s="4" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -2316,13 +2316,13 @@
         <v>19</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="D9" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="F9" s="4" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
@@ -2333,13 +2333,13 @@
         <v>5</v>
       </c>
       <c r="C10" s="3" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D10" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="F10" s="4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -2350,13 +2350,13 @@
         <v>14</v>
       </c>
       <c r="C11" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="D11" t="s">
         <v>80</v>
       </c>
-      <c r="D11" t="s">
-        <v>81</v>
-      </c>
       <c r="F11" s="4" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
@@ -2367,13 +2367,13 @@
         <v>8</v>
       </c>
       <c r="C12" s="3" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="D12" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F12" s="4" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
@@ -2384,13 +2384,13 @@
         <v>7</v>
       </c>
       <c r="C13" s="3" t="s">
+        <v>85</v>
+      </c>
+      <c r="D13" t="s">
         <v>86</v>
       </c>
-      <c r="D13" t="s">
-        <v>87</v>
-      </c>
       <c r="F13" s="4" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
@@ -2404,10 +2404,10 @@
         <v>10</v>
       </c>
       <c r="D14" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="F14" s="4" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
@@ -2421,10 +2421,10 @@
         <v>12</v>
       </c>
       <c r="D15" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="E15" s="11" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
@@ -2435,35 +2435,35 @@
         <v>13</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="D16" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="E16" s="11" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B20" t="s">
+        <v>171</v>
+      </c>
+      <c r="C20" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>29</v>
-      </c>
       <c r="D20" s="3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F20" s="4" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
@@ -2471,16 +2471,16 @@
         <v>1</v>
       </c>
       <c r="B21" t="s">
+        <v>29</v>
+      </c>
+      <c r="C21" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="C21" s="3" t="s">
-        <v>31</v>
-      </c>
       <c r="D21" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="F21" s="4" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
@@ -2488,16 +2488,16 @@
         <v>1</v>
       </c>
       <c r="B22" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="D22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="F22" s="4" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
@@ -2506,7 +2506,7 @@
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="1" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="D24" s="3"/>
       <c r="F24" s="4"/>
@@ -2522,13 +2522,13 @@
         <v>27</v>
       </c>
       <c r="D25" s="3" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="E25" s="14" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="F25" s="4" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
@@ -2537,7 +2537,7 @@
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="D27" s="3"/>
       <c r="F27" s="4"/>
@@ -2550,13 +2550,13 @@
         <v>20</v>
       </c>
       <c r="C28" s="3" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="D28" s="3" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="F28" s="4" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
@@ -2570,10 +2570,10 @@
         <v>22</v>
       </c>
       <c r="D29" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="F29" s="4" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
@@ -2584,13 +2584,13 @@
         <v>23</v>
       </c>
       <c r="C30" s="3" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="D30" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="F30" s="4" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
@@ -2601,13 +2601,13 @@
         <v>24</v>
       </c>
       <c r="C31" s="3" t="s">
+        <v>110</v>
+      </c>
+      <c r="D31" s="3" t="s">
         <v>111</v>
       </c>
-      <c r="D31" s="3" t="s">
-        <v>112</v>
-      </c>
       <c r="F31" s="4" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
@@ -2618,18 +2618,18 @@
         <v>25</v>
       </c>
       <c r="C32" s="3" t="s">
+        <v>113</v>
+      </c>
+      <c r="D32" s="3" t="s">
         <v>114</v>
       </c>
-      <c r="D32" s="3" t="s">
-        <v>115</v>
-      </c>
       <c r="F32" s="12" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A34" s="1" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
@@ -2637,16 +2637,16 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
+        <v>31</v>
+      </c>
+      <c r="C35" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C35" s="3" t="s">
-        <v>33</v>
-      </c>
       <c r="D35" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F35" s="4" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
@@ -2654,16 +2654,16 @@
         <v>4</v>
       </c>
       <c r="B36" t="s">
+        <v>33</v>
+      </c>
+      <c r="C36" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="3" t="s">
-        <v>35</v>
-      </c>
       <c r="D36" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F36" s="4" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
@@ -2671,16 +2671,16 @@
         <v>3</v>
       </c>
       <c r="B37" t="s">
+        <v>35</v>
+      </c>
+      <c r="C37" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="C37" s="3" t="s">
-        <v>37</v>
-      </c>
       <c r="D37" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F37" s="4" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
@@ -2688,16 +2688,16 @@
         <v>2</v>
       </c>
       <c r="B38" t="s">
+        <v>37</v>
+      </c>
+      <c r="C38" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="C38" s="3" t="s">
-        <v>39</v>
-      </c>
       <c r="D38" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F38" s="4" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
@@ -2705,16 +2705,16 @@
         <v>1</v>
       </c>
       <c r="B39" t="s">
+        <v>39</v>
+      </c>
+      <c r="C39" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="C39" s="3" t="s">
-        <v>41</v>
-      </c>
       <c r="D39" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F39" s="4" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
@@ -2722,16 +2722,16 @@
         <v>1</v>
       </c>
       <c r="B40" t="s">
+        <v>41</v>
+      </c>
+      <c r="C40" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="C40" s="3" t="s">
-        <v>43</v>
-      </c>
       <c r="D40" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F40" s="4" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
@@ -2739,16 +2739,16 @@
         <v>1</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" s="3">
         <v>100</v>
       </c>
       <c r="D41" s="13" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F41" s="4" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
@@ -2756,16 +2756,16 @@
         <v>1</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" s="3" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D42" s="3" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="F42" s="4" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
@@ -2773,16 +2773,16 @@
         <v>1</v>
       </c>
       <c r="B43" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C43" s="3">
         <v>470</v>
       </c>
       <c r="D43" s="3" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="F43" s="4" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
@@ -2790,19 +2790,19 @@
         <v>5</v>
       </c>
       <c r="B45" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C45" s="3" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="D45" s="13" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E45" s="14" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="F45" s="4" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
@@ -2810,19 +2810,19 @@
         <v>2</v>
       </c>
       <c r="B46" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="C46" s="3" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="D46" s="13" t="s">
+        <v>137</v>
+      </c>
+      <c r="E46" s="14" t="s">
         <v>138</v>
       </c>
-      <c r="E46" s="14" t="s">
-        <v>139</v>
-      </c>
       <c r="F46" s="4" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
   </sheetData>

</xml_diff>